<commit_message>
Work on the locations
</commit_message>
<xml_diff>
--- a/LocationOrder.xlsx
+++ b/LocationOrder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Trainer Tournament\TrainerTournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DF88DD-1CC0-4D9D-A631-E76E036F83D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E50077-E906-4F4A-B7C5-1CFB115ED904}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="4695" windowWidth="21600" windowHeight="11505" activeTab="3" xr2:uid="{7A53F6FE-011D-4876-98CD-4FEBF00B79D2}"/>
+    <workbookView xWindow="0" yWindow="4665" windowWidth="21600" windowHeight="11505" activeTab="6" xr2:uid="{7A53F6FE-011D-4876-98CD-4FEBF00B79D2}"/>
   </bookViews>
   <sheets>
     <sheet name="kanto" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="546">
   <si>
     <t>%SURF%</t>
   </si>
@@ -1253,9 +1253,6 @@
     <t>Lost_Hotel</t>
   </si>
   <si>
-    <t>Lumiose_City</t>
-  </si>
-  <si>
     <t>Lumiose_Gym</t>
   </si>
   <si>
@@ -1641,6 +1638,48 @@
   </si>
   <si>
     <t>Sendoff_Spring</t>
+  </si>
+  <si>
+    <t>Unova_Route_19</t>
+  </si>
+  <si>
+    <t>Skyarrow_Bridge</t>
+  </si>
+  <si>
+    <t>Rival battle after gym, plus Burgh is easy</t>
+  </si>
+  <si>
+    <t>ELESA!!!</t>
+  </si>
+  <si>
+    <t>Driftviel_Drawbridge</t>
+  </si>
+  <si>
+    <t>Rumination_Field</t>
+  </si>
+  <si>
+    <t>Guide says do P2 lab before Twist Mtn.  Do TM first to make it easier.</t>
+  </si>
+  <si>
+    <t>For B2W2 Gyms, only count the first boss trainer</t>
+  </si>
+  <si>
+    <t>Driftveil_Drawbridge</t>
+  </si>
+  <si>
+    <t>Reversal_Mountain</t>
+  </si>
+  <si>
+    <t>Geosenge_Town</t>
+  </si>
+  <si>
+    <t>Manually split bosses from the JSON</t>
+  </si>
+  <si>
+    <t>Boss only</t>
+  </si>
+  <si>
+    <t>Trainer only</t>
   </si>
 </sst>
 </file>
@@ -2631,7 +2670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B058CF0A-CE3D-4F41-B43B-6B7D20D55776}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -3074,7 +3113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA4260D-8524-4D6D-955B-F9FED2E65906}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -3146,7 +3185,7 @@
         <v>202</v>
       </c>
       <c r="D11" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3190,7 +3229,7 @@
         <v>209</v>
       </c>
       <c r="D18" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3295,7 +3334,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3351,7 +3390,7 @@
         <v>237</v>
       </c>
       <c r="E40" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3401,7 +3440,7 @@
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.25">
@@ -3424,7 +3463,7 @@
         <v>216</v>
       </c>
       <c r="E54" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.25">
@@ -3439,7 +3478,7 @@
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.25">
@@ -3449,7 +3488,7 @@
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.25">
@@ -3469,12 +3508,12 @@
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="64" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
@@ -3519,10 +3558,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E930C9-DAC1-4257-BBDD-97CF3AD7AF71}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A49" sqref="A1:B49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3530,383 +3569,408 @@
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66.28515625" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>276</v>
       </c>
       <c r="B6" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>277</v>
-      </c>
-      <c r="B7" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>278</v>
       </c>
-      <c r="B8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>279</v>
       </c>
-      <c r="B9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>280</v>
       </c>
-      <c r="B10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>281</v>
       </c>
       <c r="B11" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>282</v>
       </c>
       <c r="B12" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>283</v>
-      </c>
-      <c r="B13" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D12" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>284</v>
       </c>
-      <c r="B14" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>285</v>
       </c>
-      <c r="B15" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>286</v>
-      </c>
-      <c r="B16" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>287</v>
-      </c>
-      <c r="B17" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>283</v>
+      </c>
+      <c r="E15" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>288</v>
       </c>
-      <c r="B18" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D18" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>312</v>
+      </c>
+      <c r="E19" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>289</v>
       </c>
-      <c r="B19" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>290</v>
-      </c>
-      <c r="B20" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>291</v>
-      </c>
-      <c r="B21" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>292</v>
-      </c>
-      <c r="B22" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>335</v>
+      </c>
+      <c r="D23" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>336</v>
+      </c>
+      <c r="D24" t="s">
         <v>293</v>
       </c>
-      <c r="B23" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>294</v>
-      </c>
-      <c r="B24" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>295</v>
       </c>
       <c r="B25" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+      <c r="D25" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>296</v>
       </c>
       <c r="B26" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+      <c r="D26" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>297</v>
       </c>
       <c r="B27" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+      <c r="D27" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>298</v>
       </c>
       <c r="B28" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+      <c r="D28" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>299</v>
       </c>
-      <c r="B29" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>300</v>
-      </c>
-      <c r="B30" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>301</v>
       </c>
       <c r="B31" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>532</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>302</v>
       </c>
       <c r="B32" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+      <c r="D32" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>303</v>
       </c>
       <c r="B33" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+      <c r="D33" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>304</v>
       </c>
       <c r="B34" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+        <v>346</v>
+      </c>
+      <c r="D34" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>347</v>
+      </c>
+      <c r="D35" t="s">
         <v>305</v>
       </c>
-      <c r="B35" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>306</v>
-      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>307</v>
-      </c>
-      <c r="B37" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>308</v>
       </c>
       <c r="B38" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>309</v>
-      </c>
+      <c r="D38" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>310</v>
-      </c>
+      <c r="D39" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>311</v>
-      </c>
+      <c r="D40" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>312</v>
-      </c>
-      <c r="B42" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>313</v>
       </c>
       <c r="B43" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>314</v>
       </c>
       <c r="B44" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="D44" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>319</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3916,10 +3980,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34571B6-E3D8-40E3-B225-D44DA32A91BD}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection sqref="A1:B49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3929,381 +3993,398 @@
     <col min="4" max="4" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>532</v>
+      </c>
+      <c r="E1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>276</v>
       </c>
-      <c r="B6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>277</v>
       </c>
       <c r="B7" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>278</v>
       </c>
       <c r="B8" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>279</v>
-      </c>
+      <c r="D8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>280</v>
       </c>
       <c r="B10" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>281</v>
       </c>
-      <c r="B11" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>282</v>
       </c>
-      <c r="B12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>283</v>
-      </c>
-      <c r="B13" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>284</v>
-      </c>
+      <c r="D12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>285</v>
-      </c>
+      <c r="D14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="D15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>286</v>
       </c>
       <c r="B16" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>287</v>
-      </c>
-      <c r="B17" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="D16" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>288</v>
       </c>
       <c r="B18" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+      <c r="D18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>289</v>
       </c>
-      <c r="B19" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>290</v>
-      </c>
-      <c r="B20" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>291</v>
       </c>
       <c r="B21" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="D21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>292</v>
       </c>
-      <c r="B22" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>293</v>
-      </c>
+      <c r="D22" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>294</v>
-      </c>
-      <c r="B24" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>295</v>
-      </c>
-      <c r="B25" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>296</v>
       </c>
-      <c r="B26" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>297</v>
-      </c>
+      <c r="D26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>298</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="D27" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+      <c r="D28" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>299</v>
       </c>
-      <c r="B29" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>300</v>
       </c>
       <c r="B30" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>301</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="D30" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="D31" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>302</v>
       </c>
-      <c r="B32" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>303</v>
-      </c>
-      <c r="B33" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>304</v>
       </c>
-      <c r="B34" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>305</v>
       </c>
-      <c r="B35" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>306</v>
-      </c>
-      <c r="B36" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>307</v>
       </c>
       <c r="B37" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>308</v>
       </c>
-      <c r="B38" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>309</v>
       </c>
-      <c r="B39" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>310</v>
       </c>
-      <c r="B40" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>311</v>
-      </c>
-      <c r="B41" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>312</v>
-      </c>
+      <c r="D40" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>313</v>
       </c>
       <c r="B43" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>314</v>
-      </c>
+      <c r="D43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>319</v>
+      </c>
+      <c r="D49" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4313,10 +4394,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB38F73-5919-446D-B66E-AADED71FD445}">
-  <dimension ref="A1:A59"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AO57" sqref="AO57"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4325,299 +4406,316 @@
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C19" t="s">
+        <v>542</v>
+      </c>
+      <c r="E19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>415</v>
+      </c>
+      <c r="E24" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>414</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C42" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>542</v>
+      </c>
+      <c r="E46" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>417</v>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4666,112 +4764,112 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -4781,187 +4879,187 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -5009,232 +5107,232 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wild data is parsing correctly
</commit_message>
<xml_diff>
--- a/LocationOrder.xlsx
+++ b/LocationOrder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Trainer Tournament\TrainerTournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E50077-E906-4F4A-B7C5-1CFB115ED904}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130CEBED-9D48-4882-A4FC-BCDE6891B1DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4665" windowWidth="21600" windowHeight="11505" activeTab="6" xr2:uid="{7A53F6FE-011D-4876-98CD-4FEBF00B79D2}"/>
+    <workbookView xWindow="21435" yWindow="5745" windowWidth="21600" windowHeight="11505" activeTab="8" xr2:uid="{7A53F6FE-011D-4876-98CD-4FEBF00B79D2}"/>
   </bookViews>
   <sheets>
     <sheet name="kanto" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="557">
   <si>
     <t>%SURF%</t>
   </si>
@@ -386,9 +386,6 @@
     <t>%FORCE%</t>
   </si>
   <si>
-    <t>Tohjo_Fals</t>
-  </si>
-  <si>
     <t>Abandoned_Ship</t>
   </si>
   <si>
@@ -1680,6 +1677,42 @@
   </si>
   <si>
     <t>Trainer only</t>
+  </si>
+  <si>
+    <t>Ten_Carat_Hill</t>
+  </si>
+  <si>
+    <t>Alola_Route_5</t>
+  </si>
+  <si>
+    <t>Brooklet_Hill</t>
+  </si>
+  <si>
+    <t>Lush_Jungle</t>
+  </si>
+  <si>
+    <t>Visit multiple times</t>
+  </si>
+  <si>
+    <t>Alola_Route_13</t>
+  </si>
+  <si>
+    <t>Thrifty_Megamart_(Abandoned_Site)</t>
+  </si>
+  <si>
+    <t>Ula%27ula_Meadow</t>
+  </si>
+  <si>
+    <t>Galar_Route_1</t>
+  </si>
+  <si>
+    <t>Leon only</t>
+  </si>
+  <si>
+    <t>Semifinals</t>
+  </si>
+  <si>
+    <t>Finals</t>
   </si>
 </sst>
 </file>
@@ -2038,7 +2071,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView zoomScale="63" workbookViewId="0">
-      <selection activeCell="C54" sqref="C53:C54"/>
+      <selection activeCell="C55" sqref="C1:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,7 +2386,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C58" sqref="C1:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,7 +2666,7 @@
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
@@ -2671,7 +2704,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E75" sqref="E1:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,58 +2717,58 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
@@ -2745,144 +2778,144 @@
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
@@ -2897,71 +2930,71 @@
     </row>
     <row r="37" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="5:5" x14ac:dyDescent="0.25">
@@ -2971,128 +3004,128 @@
     </row>
     <row r="51" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F69" s="2"/>
     </row>
     <row r="70" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F70" s="2"/>
     </row>
     <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F71" s="2"/>
     </row>
     <row r="72" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="5:6" x14ac:dyDescent="0.25">
@@ -3113,8 +3146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA4260D-8524-4D6D-955B-F9FED2E65906}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3126,22 +3159,22 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3149,25 +3182,25 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3177,97 +3210,97 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D11" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D18" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
@@ -3275,127 +3308,127 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E40" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3405,145 +3438,145 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E54" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="64" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.25">
@@ -3561,7 +3594,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="D49" sqref="D1:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3574,7 +3607,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3582,10 +3615,10 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3593,10 +3626,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3604,370 +3637,370 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E15" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B31" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D31" t="s">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B32" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D35" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D36" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B38" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D38" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D39" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D40" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B43" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D43" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B44" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D44" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
@@ -3983,7 +4016,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="D1" sqref="D1:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3995,10 +4028,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4006,7 +4039,7 @@
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4014,10 +4047,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4025,162 +4058,162 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
@@ -4188,198 +4221,198 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D28" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B30" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D37" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D38" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D39" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D40" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D42" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B43" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D43" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D44" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D46" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D47" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D49" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4396,8 +4429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB38F73-5919-446D-B66E-AADED71FD445}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4408,78 +4441,78 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4489,64 +4522,64 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E24" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
@@ -4554,12 +4587,12 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -4569,57 +4602,57 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -4629,88 +4662,88 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C42" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E46" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
@@ -4725,10 +4758,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7503DAE6-4D1B-4F80-9E90-95ADC34463B4}">
-  <dimension ref="A1:A65"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AI51" sqref="AI51"/>
+      <selection activeCell="C50" sqref="C1:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4737,329 +4770,345 @@
     <col min="3" max="3" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>418</v>
+      </c>
+      <c r="C8" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>436</v>
+      </c>
+      <c r="C26" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>437</v>
+      </c>
+      <c r="C27" t="s">
+        <v>417</v>
+      </c>
+      <c r="E27" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>439</v>
+      </c>
+      <c r="C30" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>440</v>
+      </c>
+      <c r="C31" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>444</v>
+      </c>
+      <c r="C35" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>445</v>
+      </c>
+      <c r="C36" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>447</v>
+      </c>
+      <c r="C38" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>448</v>
+      </c>
+      <c r="C39" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>449</v>
+      </c>
+      <c r="C40" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>417</v>
+      </c>
+      <c r="E42" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>457</v>
+      </c>
+      <c r="C48" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>458</v>
+      </c>
+      <c r="C49" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>459</v>
+      </c>
+      <c r="C50" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>472</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -5069,270 +5118,271 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC3A95F-195D-4DDF-987C-2B6DC96E800F}">
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C33" sqref="C1:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C3" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>475</v>
+      </c>
+      <c r="C6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>478</v>
+      </c>
+      <c r="C9" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>481</v>
+      </c>
+      <c r="C12" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>483</v>
+      </c>
+      <c r="C14" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>495</v>
+      </c>
+      <c r="C26" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>520</v>
+      </c>
+      <c r="E27" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>497</v>
+      </c>
+      <c r="C28" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>520</v>
+      </c>
+      <c r="E30" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>500</v>
+      </c>
+      <c r="C31" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>501</v>
+      </c>
+      <c r="C32" t="s">
+        <v>520</v>
+      </c>
+      <c r="E32" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>502</v>
+      </c>
+      <c r="C33" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>517</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>